<commit_message>
Crushed out roughly 50% of numba re-implementation, and provided valid tests via ChartSchool data
</commit_message>
<xml_diff>
--- a/resources/cs-ema.xlsx
+++ b/resources/cs-ema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2020EBF1-F492-4CF0-AB6E-26EBFC73597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A85B65E-92AA-45C5-9765-8FDB5A42B7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="-10065" windowWidth="15315" windowHeight="12960" xr2:uid="{D1679BA8-4038-48BD-921F-8BB061D5560D}"/>
+    <workbookView xWindow="28950" yWindow="2475" windowWidth="15615" windowHeight="12960" xr2:uid="{D1679BA8-4038-48BD-921F-8BB061D5560D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>